<commit_message>
Diversas Correções para rodar a Xalingo
</commit_message>
<xml_diff>
--- a/tests/testesmanuais/CBA_SESI_Planilha_Dados_Entrada - v1.1 - Versão Completa.xlsx
+++ b/tests/testesmanuais/CBA_SESI_Planilha_Dados_Entrada - v1.1 - Versão Completa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="846" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="846" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pl. suporte" sheetId="51" state="hidden" r:id="rId1"/>
@@ -5082,7 +5082,7 @@
   </sheetPr>
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8732,8 +8732,8 @@
   </sheetPr>
   <dimension ref="A1:T87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C19" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="N12" sqref="J12:N12"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12583,8 +12583,8 @@
   </sheetPr>
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14544,9 +14544,7 @@
   </sheetPr>
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21:N21"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>